<commit_message>
FS and KZN updates
</commit_message>
<xml_diff>
--- a/applications/south_africa/FS_projections.xlsx
+++ b/applications/south_africa/FS_projections.xlsx
@@ -584,76 +584,76 @@
     </row>
     <row r="4" spans="1:24">
       <c r="A4">
-        <v>54258</v>
+        <v>37530</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>845</v>
       </c>
       <c r="C4">
-        <v>54258</v>
+        <v>97042</v>
       </c>
       <c r="D4">
-        <v>1.288643616556319</v>
+        <v>0.8913436097821972</v>
       </c>
       <c r="E4">
-        <v>0.0003116184806358656</v>
+        <v>0.02007217454637576</v>
       </c>
       <c r="F4">
-        <v>1.288643616556319</v>
+        <v>2.304756198585654</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>0.2233735931670334</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.01324390892681846</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>0.3589482933770215</v>
       </c>
       <c r="J4">
-        <v>0.03255109168076911</v>
+        <v>0.02860994820120611</v>
       </c>
       <c r="K4">
-        <v>0.01021963146394756</v>
+        <v>0.009342840495265839</v>
       </c>
       <c r="L4">
-        <v>0.03255109168076911</v>
+        <v>0.05376641014642117</v>
       </c>
       <c r="M4">
-        <v>598679</v>
+        <v>323153</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>263</v>
       </c>
       <c r="O4">
-        <v>598679</v>
+        <v>682982</v>
       </c>
       <c r="P4">
-        <v>14.86490926992368</v>
+        <v>8.023739693690269</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>0.006552486261007747</v>
       </c>
       <c r="R4">
-        <v>14.86490926992368</v>
+        <v>16.95812267353212</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>0.5169970601880156</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>0.004890021849963582</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>0.6714657200384131</v>
       </c>
       <c r="V4">
-        <v>0.6511681657863504</v>
+        <v>0.2227171165814395</v>
       </c>
       <c r="W4">
-        <v>0.01021963146394756</v>
+        <v>0.009465147851420249</v>
       </c>
       <c r="X4">
-        <v>0.6511681657863504</v>
+        <v>0.4669746120339427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>